<commit_message>
Corrected error in student  test data 2
</commit_message>
<xml_diff>
--- a/test_data/td_2_students.xlsx
+++ b/test_data/td_2_students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hertieschool-my.sharepoint.com/personal/234533_students_hertie-school_org/Documents/MDS/DSA/student-project-matching/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE52CC27-FFB6-AB4E-B81F-1CD9CFF4E9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{FE52CC27-FFB6-AB4E-B81F-1CD9CFF4E9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{223B28B5-FE6C-DA4B-9FF6-22634957C458}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{167CAB08-E6E9-D544-8315-BD75E8338A04}"/>
   </bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,7 +477,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>